<commit_message>
Definitive datadictionary en database ontwerp aanpassingen
</commit_message>
<xml_diff>
--- a/Project documents/elaboration-phase/20161016_genormaliseerde database_structuur.xlsx
+++ b/Project documents/elaboration-phase/20161016_genormaliseerde database_structuur.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
   <si>
     <t>Customer_ID</t>
   </si>
@@ -210,6 +210,33 @@
   </si>
   <si>
     <t>•Quotation_ID</t>
+  </si>
+  <si>
+    <t>Ledger account number</t>
+  </si>
+  <si>
+    <t>Hardware and software</t>
+  </si>
+  <si>
+    <t>•Maintenace contract</t>
+  </si>
+  <si>
+    <t>•Hardware and software</t>
+  </si>
+  <si>
+    <t>Maintenance contract</t>
+  </si>
+  <si>
+    <t>Project_ID</t>
+  </si>
+  <si>
+    <t>• Paid</t>
+  </si>
+  <si>
+    <t>•Paid</t>
+  </si>
+  <si>
+    <t>Paid</t>
   </si>
 </sst>
 </file>
@@ -590,18 +617,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M80"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="21.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
@@ -702,430 +729,484 @@
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>24</v>
+      <c r="B21" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>38</v>
+      <c r="B25" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>39</v>
+      <c r="B26" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D50" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D68" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
+      <c r="D76" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
+      <c r="D77" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D58" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D59" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D63" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J63" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H66" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H67" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="1" t="s">
-        <v>15</v>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>